<commit_message>
Results Updated and PathEnrResults Added
</commit_message>
<xml_diff>
--- a/Results/Results_with_RobustRankAggreg_Package_Ranking_Strategy/THCA/miRcorrNet Results/THCA_mRNA_miRcorrNet_res1.xlsx
+++ b/Results/Results_with_RobustRankAggreg_Package_Ranking_Strategy/THCA/miRcorrNet Results/THCA_mRNA_miRcorrNet_res1.xlsx
@@ -173,58 +173,58 @@
         <v>10.0</v>
       </c>
       <c r="B2" t="n">
-        <v>257.40659340659323</v>
+        <v>253.96551724137922</v>
       </c>
       <c r="C2" t="n">
-        <v>0.964590964590964</v>
+        <v>0.9693486590038315</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9542124542124543</v>
+        <v>0.9616858237547893</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9697802197802199</v>
+        <v>0.9731800766283526</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9481110464626947</v>
+        <v>0.9547456375042581</v>
       </c>
       <c r="G2" t="n">
-        <v>0.996336996336996</v>
+        <v>0.9951309067688379</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9542124542124543</v>
+        <v>0.9616858237547893</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9503401360544218</v>
+        <v>0.955322933771209</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9215142669084376</v>
+        <v>0.9317821508826001</v>
       </c>
       <c r="K2" t="n">
-        <v>98.2813397030267</v>
+        <v>84.32515256584249</v>
       </c>
       <c r="L2" t="n">
-        <v>0.042646088398906205</v>
+        <v>0.04129560937376906</v>
       </c>
       <c r="M2" t="n">
-        <v>0.07882600806125035</v>
+        <v>0.07916370629017346</v>
       </c>
       <c r="N2" t="n">
-        <v>0.05626832145583103</v>
+        <v>0.05002301291071051</v>
       </c>
       <c r="O2" t="n">
-        <v>0.07882600806125035</v>
+        <v>0.07916370629017346</v>
       </c>
       <c r="P2" t="n">
-        <v>0.08504928056448624</v>
+        <v>0.08047560872662458</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.05976270207289693</v>
+        <v>0.05987099927422121</v>
       </c>
       <c r="R2" t="n">
-        <v>0.09187241359684008</v>
+        <v>0.09071061184605762</v>
       </c>
       <c r="S2" t="n">
-        <v>0.008682293612399824</v>
+        <v>0.012669100181615926</v>
       </c>
       <c r="T2" t="n">
         <v>9.0</v>
@@ -240,58 +240,58 @@
         <v>9.0</v>
       </c>
       <c r="B3" t="n">
-        <v>242.73195876288668</v>
+        <v>239.89108910891093</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9650630011454747</v>
+        <v>0.9735973597359733</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9570446735395186</v>
+        <v>0.9653465346534653</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9690721649484535</v>
+        <v>0.9777227722772274</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9491455280115072</v>
+        <v>0.9610600620501611</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9967783505154637</v>
+        <v>0.9942244224422438</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9570446735395186</v>
+        <v>0.9653465346534653</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9496072655866468</v>
+        <v>0.9629302215935874</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9228374658361207</v>
+        <v>0.9412521787295782</v>
       </c>
       <c r="K3" t="n">
-        <v>95.99994742445583</v>
+        <v>76.82628469346922</v>
       </c>
       <c r="L3" t="n">
-        <v>0.04341959868782073</v>
+        <v>0.03896346769966366</v>
       </c>
       <c r="M3" t="n">
-        <v>0.07712405274143289</v>
+        <v>0.07194454532318967</v>
       </c>
       <c r="N3" t="n">
-        <v>0.05808427439864016</v>
+        <v>0.046979737223297936</v>
       </c>
       <c r="O3" t="n">
-        <v>0.07712405274143289</v>
+        <v>0.07194454532318967</v>
       </c>
       <c r="P3" t="n">
-        <v>0.08651363414075097</v>
+        <v>0.07559233772144715</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.06012343075255459</v>
+        <v>0.055872217072821</v>
       </c>
       <c r="R3" t="n">
-        <v>0.09294503005974018</v>
+        <v>0.08521684068884133</v>
       </c>
       <c r="S3" t="n">
-        <v>0.008146897900310531</v>
+        <v>0.01546817306039549</v>
       </c>
       <c r="T3" t="n">
         <v>9.0</v>
@@ -307,58 +307,58 @@
         <v>8.0</v>
       </c>
       <c r="B4" t="n">
-        <v>227.93577981651387</v>
+        <v>228.11650485436905</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9704383282364936</v>
+        <v>0.9746494066882411</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9633027522935778</v>
+        <v>0.9660194174757281</v>
       </c>
       <c r="E4" t="n">
-        <v>0.974006116207951</v>
+        <v>0.9789644012944982</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9566859745758831</v>
+        <v>0.9624563139126245</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9971330275229358</v>
+        <v>0.9948759439050695</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9633027522935778</v>
+        <v>0.9660194174757281</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9573394495412841</v>
+        <v>0.9648636153490522</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9344782819892515</v>
+        <v>0.9434683425481231</v>
       </c>
       <c r="K4" t="n">
-        <v>91.89056244909118</v>
+        <v>78.59979306599435</v>
       </c>
       <c r="L4" t="n">
-        <v>0.03896876521972285</v>
+        <v>0.03712682392526563</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0729937358674962</v>
+        <v>0.07139759223530995</v>
       </c>
       <c r="N4" t="n">
-        <v>0.05159150210855409</v>
+        <v>0.04476768677440194</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0729937358674962</v>
+        <v>0.07139759223530995</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0782347608088152</v>
+        <v>0.07314652532981213</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.054759368259657264</v>
+        <v>0.05426269315081091</v>
       </c>
       <c r="R4" t="n">
-        <v>0.08405360685676078</v>
+        <v>0.08204729164060874</v>
       </c>
       <c r="S4" t="n">
-        <v>0.007147932328715096</v>
+        <v>0.014649681944059462</v>
       </c>
       <c r="T4" t="n">
         <v>9.0</v>
@@ -374,58 +374,58 @@
         <v>7.0</v>
       </c>
       <c r="B5" t="n">
-        <v>217.42718446601936</v>
+        <v>211.13761467889918</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9681769147788566</v>
+        <v>0.9765545361875636</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9627831715210357</v>
+        <v>0.9663608562691128</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9708737864077672</v>
+        <v>0.9816513761467887</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9532050473798048</v>
+        <v>0.9650102191386597</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9962243797195254</v>
+        <v>0.9949031600407747</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9627831715210357</v>
+        <v>0.9663608562691128</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9511095700416088</v>
+        <v>0.9688728702490171</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9292776746259231</v>
+        <v>0.9475046652589532</v>
       </c>
       <c r="K5" t="n">
-        <v>90.52489657999384</v>
+        <v>71.47823650774801</v>
       </c>
       <c r="L5" t="n">
-        <v>0.03615670135993209</v>
+        <v>0.03648788718412104</v>
       </c>
       <c r="M5" t="n">
-        <v>0.07355003200936898</v>
+        <v>0.07092791983137557</v>
       </c>
       <c r="N5" t="n">
-        <v>0.04769858423390126</v>
+        <v>0.04144663844159234</v>
       </c>
       <c r="O5" t="n">
-        <v>0.07355003200936898</v>
+        <v>0.07092791983137557</v>
       </c>
       <c r="P5" t="n">
-        <v>0.07790283363790781</v>
+        <v>0.06886394290698962</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.052830017179578775</v>
+        <v>0.05387912599358178</v>
       </c>
       <c r="R5" t="n">
-        <v>0.07985408674594387</v>
+        <v>0.08109649833982617</v>
       </c>
       <c r="S5" t="n">
-        <v>0.00782639613981815</v>
+        <v>0.014444957658776687</v>
       </c>
       <c r="T5" t="n">
         <v>9.0</v>
@@ -441,58 +441,58 @@
         <v>6.0</v>
       </c>
       <c r="B6" t="n">
-        <v>208.8</v>
+        <v>200.24000000000018</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9644444444444442</v>
+        <v>0.9755555555555552</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9583333333333331</v>
+        <v>0.9649999999999999</v>
       </c>
       <c r="E6" t="n">
+        <v>0.9808333333333327</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.9637212787212788</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.995486111111111</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9649999999999999</v>
+      </c>
+      <c r="I6" t="n">
         <v>0.9674999999999999</v>
       </c>
-      <c r="F6" t="n">
-        <v>0.9482419247419249</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.9963194444444443</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.9583333333333331</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.9467142857142856</v>
-      </c>
       <c r="J6" t="n">
-        <v>0.9214556863426429</v>
+        <v>0.9454030100334446</v>
       </c>
       <c r="K6" t="n">
-        <v>81.45681138623166</v>
+        <v>72.32797354810765</v>
       </c>
       <c r="L6" t="n">
-        <v>0.041423721210062464</v>
+        <v>0.03646015374110923</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0763027521703925</v>
+        <v>0.06822669679005593</v>
       </c>
       <c r="N6" t="n">
-        <v>0.056674340934090565</v>
+        <v>0.0424670599223677</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0763027521703925</v>
+        <v>0.06822669679005593</v>
       </c>
       <c r="P6" t="n">
-        <v>0.08486956158597411</v>
+        <v>0.07047737265495682</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.05734656558963597</v>
+        <v>0.05296267831786668</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0886261082053257</v>
+        <v>0.0804535837704723</v>
       </c>
       <c r="S6" t="n">
-        <v>0.007924342076302805</v>
+        <v>0.014076143687523917</v>
       </c>
       <c r="T6" t="n">
         <v>5.0</v>
@@ -508,58 +508,58 @@
         <v>5.0</v>
       </c>
       <c r="B7" t="n">
-        <v>186.57000000000008</v>
+        <v>180.63999999999996</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9638888888888887</v>
+        <v>0.9766666666666667</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9566666666666668</v>
+        <v>0.9666666666666665</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9675</v>
+        <v>0.9816666666666665</v>
       </c>
       <c r="F7" t="n">
-        <v>0.947454378954379</v>
+        <v>0.9650729270729269</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9963888888888885</v>
+        <v>0.9956249999999995</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9566666666666668</v>
+        <v>0.9666666666666665</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9468333333333334</v>
+        <v>0.9692857142857142</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9202479940349505</v>
+        <v>0.9476834296138642</v>
       </c>
       <c r="K7" t="n">
-        <v>77.37136669232605</v>
+        <v>69.69913988716146</v>
       </c>
       <c r="L7" t="n">
-        <v>0.04279704989525579</v>
+        <v>0.033668350126272215</v>
       </c>
       <c r="M7" t="n">
-        <v>0.07719841941125288</v>
+        <v>0.07106690545187216</v>
       </c>
       <c r="N7" t="n">
-        <v>0.057898814558438115</v>
+        <v>0.04030606808631133</v>
       </c>
       <c r="O7" t="n">
-        <v>0.07719841941125288</v>
+        <v>0.07106690545187216</v>
       </c>
       <c r="P7" t="n">
-        <v>0.08665512651181428</v>
+        <v>0.06657770811845104</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.059271187917323116</v>
+        <v>0.04997485691631375</v>
       </c>
       <c r="R7" t="n">
-        <v>0.09162071749866367</v>
+        <v>0.07496879081790679</v>
       </c>
       <c r="S7" t="n">
-        <v>0.008286437444157559</v>
+        <v>0.013485117112067268</v>
       </c>
       <c r="T7" t="n">
         <v>4.0</v>
@@ -575,58 +575,58 @@
         <v>4.0</v>
       </c>
       <c r="B8" t="n">
-        <v>160.74000000000007</v>
+        <v>158.82000000000002</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9666666666666665</v>
+        <v>0.9761111111111106</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9550000000000001</v>
+        <v>0.9649999999999997</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9725000000000001</v>
+        <v>0.9816666666666665</v>
       </c>
       <c r="F8" t="n">
-        <v>0.950891441891442</v>
+        <v>0.9640772560772557</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9961111111111108</v>
+        <v>0.9952777777777773</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9550000000000001</v>
+        <v>0.9649999999999997</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9546428571428571</v>
+        <v>0.9684523809523807</v>
       </c>
       <c r="J8" t="n">
-        <v>0.9258960271612446</v>
+        <v>0.9462954697476436</v>
       </c>
       <c r="K8" t="n">
-        <v>71.93046867101816</v>
+        <v>73.35817485585241</v>
       </c>
       <c r="L8" t="n">
-        <v>0.04103049699312549</v>
+        <v>0.03464947485885504</v>
       </c>
       <c r="M8" t="n">
-        <v>0.07804787157979805</v>
+        <v>0.07222222222222482</v>
       </c>
       <c r="N8" t="n">
-        <v>0.05304292779015674</v>
+        <v>0.03852644958492143</v>
       </c>
       <c r="O8" t="n">
-        <v>0.07804787157979805</v>
+        <v>0.07222222222222482</v>
       </c>
       <c r="P8" t="n">
-        <v>0.08222994874191568</v>
+        <v>0.06565086674282744</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.0585094435221705</v>
+        <v>0.05194011360887088</v>
       </c>
       <c r="R8" t="n">
-        <v>0.08935178870625705</v>
+        <v>0.07761785866715273</v>
       </c>
       <c r="S8" t="n">
-        <v>0.010032914406692364</v>
+        <v>0.012977985523274735</v>
       </c>
       <c r="T8" t="n">
         <v>3.0</v>
@@ -642,58 +642,58 @@
         <v>3.0</v>
       </c>
       <c r="B9" t="n">
-        <v>126.49999999999997</v>
+        <v>128.10000000000002</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9649999999999996</v>
+        <v>0.9733333333333328</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9566666666666666</v>
+        <v>0.9616666666666667</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9691666666666666</v>
+        <v>0.9791666666666661</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9491027306027306</v>
+        <v>0.9602707292707291</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9961111111111113</v>
+        <v>0.9952083333333329</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9566666666666666</v>
+        <v>0.9616666666666667</v>
       </c>
       <c r="I9" t="n">
-        <v>0.950047619047619</v>
+        <v>0.964880952380952</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9227403017272583</v>
+        <v>0.9403577885882232</v>
       </c>
       <c r="K9" t="n">
-        <v>68.3568326186678</v>
+        <v>65.89531029740978</v>
       </c>
       <c r="L9" t="n">
-        <v>0.04371953716495552</v>
+        <v>0.03826255278343741</v>
       </c>
       <c r="M9" t="n">
-        <v>0.07719841941125288</v>
+        <v>0.07436600722307987</v>
       </c>
       <c r="N9" t="n">
-        <v>0.05881236690153198</v>
+        <v>0.044907624352969515</v>
       </c>
       <c r="O9" t="n">
-        <v>0.07719841941125288</v>
+        <v>0.07436600722307987</v>
       </c>
       <c r="P9" t="n">
-        <v>0.08746801662096988</v>
+        <v>0.07256935351705382</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.06043485917152861</v>
+        <v>0.055814239468645326</v>
       </c>
       <c r="R9" t="n">
-        <v>0.09351863733212275</v>
+        <v>0.08440829874482399</v>
       </c>
       <c r="S9" t="n">
-        <v>0.00988618356666293</v>
+        <v>0.013558607996074425</v>
       </c>
       <c r="T9" t="n">
         <v>2.0</v>
@@ -709,58 +709,58 @@
         <v>2.0</v>
       </c>
       <c r="B10" t="n">
-        <v>85.35000000000004</v>
+        <v>90.26999999999997</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9599999999999995</v>
+        <v>0.9744444444444442</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9500000000000002</v>
+        <v>0.9616666666666668</v>
       </c>
       <c r="E10" t="n">
-        <v>0.965</v>
+        <v>0.9808333333333329</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9411162171162173</v>
+        <v>0.9613616383616387</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9950694444444445</v>
+        <v>0.993958333333333</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9500000000000002</v>
+        <v>0.9616666666666668</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9411904761904762</v>
+        <v>0.9667857142857137</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9110877064964026</v>
+        <v>0.9423867740954698</v>
       </c>
       <c r="K10" t="n">
-        <v>59.14942130235967</v>
+        <v>59.06867343878802</v>
       </c>
       <c r="L10" t="n">
-        <v>0.04258161181833561</v>
+        <v>0.03295709855904684</v>
       </c>
       <c r="M10" t="n">
-        <v>0.08375315127159834</v>
+        <v>0.07436600722307891</v>
       </c>
       <c r="N10" t="n">
-        <v>0.05451037031042474</v>
+        <v>0.0371830036115245</v>
       </c>
       <c r="O10" t="n">
-        <v>0.08375315127159834</v>
+        <v>0.07436600722307891</v>
       </c>
       <c r="P10" t="n">
-        <v>0.08705231367517363</v>
+        <v>0.06379112019502256</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.06188353179421072</v>
+        <v>0.050223581316696686</v>
       </c>
       <c r="R10" t="n">
-        <v>0.0936734420366698</v>
+        <v>0.07444368819542706</v>
       </c>
       <c r="S10" t="n">
-        <v>0.013687335239748738</v>
+        <v>0.015375510022579296</v>
       </c>
       <c r="T10" t="n">
         <v>1.0</v>
@@ -776,58 +776,58 @@
         <v>1.0</v>
       </c>
       <c r="B11" t="n">
-        <v>40.93000000000002</v>
+        <v>45.12000000000001</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9549999999999997</v>
+        <v>0.9649999999999999</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9450000000000003</v>
+        <v>0.9516666666666663</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9600000000000001</v>
+        <v>0.9716666666666665</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9334189144189142</v>
+        <v>0.9484775224775224</v>
       </c>
       <c r="G11" t="n">
-        <v>0.9911805555555553</v>
+        <v>0.9897222222222218</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9450000000000003</v>
+        <v>0.9516666666666663</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9299047619047618</v>
+        <v>0.9529166666666663</v>
       </c>
       <c r="J11" t="n">
-        <v>0.8996867031519205</v>
+        <v>0.922206283571501</v>
       </c>
       <c r="K11" t="n">
-        <v>38.55869329065533</v>
+        <v>39.832802075828425</v>
       </c>
       <c r="L11" t="n">
-        <v>0.04717681186245255</v>
+        <v>0.0444269045075346</v>
       </c>
       <c r="M11" t="n">
-        <v>0.09191502932077547</v>
+        <v>0.0796139676086065</v>
       </c>
       <c r="N11" t="n">
-        <v>0.05360201681381411</v>
+        <v>0.054561819467998825</v>
       </c>
       <c r="O11" t="n">
-        <v>0.09191502932077547</v>
+        <v>0.0796139676086065</v>
       </c>
       <c r="P11" t="n">
-        <v>0.08929080953876059</v>
+        <v>0.08601344948357957</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.07172800926629866</v>
+        <v>0.06297385193042307</v>
       </c>
       <c r="R11" t="n">
-        <v>0.10613847704019748</v>
+        <v>0.09656761895675348</v>
       </c>
       <c r="S11" t="n">
-        <v>0.0180349046627549</v>
+        <v>0.024685482606220884</v>
       </c>
       <c r="T11" t="n">
         <v>0.0</v>

</xml_diff>